<commit_message>
Fixed bug preventing optimization from working
</commit_message>
<xml_diff>
--- a/data/GroupSpec_cubic.xlsx
+++ b/data/GroupSpec_cubic.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DWMoreau/MLI/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36C98D9-DE62-DA43-AA1C-BF7492807D0B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A75EF3-81C1-5249-93AA-076E11C33163}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5540" yWindow="880" windowWidth="24700" windowHeight="16840" activeTab="2" xr2:uid="{7928E02C-29DC-574B-8667-D82DDE3DF551}"/>
+    <workbookView xWindow="5540" yWindow="880" windowWidth="24700" windowHeight="16840" xr2:uid="{7928E02C-29DC-574B-8667-D82DDE3DF551}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
     <sheet name="Groups V0" sheetId="5" r:id="rId2"/>
     <sheet name="Groups V1" sheetId="7" r:id="rId3"/>
     <sheet name="Groups V2" sheetId="6" r:id="rId4"/>
+    <sheet name="Groups V3" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1288" uniqueCount="70">
   <si>
     <t>spacegroup number</t>
   </si>
@@ -599,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23E9EF93-9C26-5E4D-979F-BFF17FE810E6}">
   <dimension ref="A1:K168"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I37" sqref="A1:K37"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2855,8 +2856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A60AFE1-6AB8-D64E-9454-61131BC5B2BC}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3988,7 +3989,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFC2BFA0-9478-3A49-B32B-95904FA22C6D}">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
@@ -4957,4 +4958,1131 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A97EA6C-E4EF-694D-8776-4A662F7FA16D}">
+  <dimension ref="A1:K43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D28" sqref="D28:K30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="27.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>195</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>200</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>207</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>215</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>221</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <f>SUM(D2:D6)</f>
+        <v>668</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>222</v>
+      </c>
+      <c r="B9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9">
+        <v>141</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" t="s">
+        <v>24</v>
+      </c>
+      <c r="K9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>223</v>
+      </c>
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10">
+        <v>115</v>
+      </c>
+      <c r="I10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" t="s">
+        <v>24</v>
+      </c>
+      <c r="K10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>224</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11">
+        <v>38</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" t="s">
+        <v>24</v>
+      </c>
+      <c r="K11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>218</v>
+      </c>
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12">
+        <v>171</v>
+      </c>
+      <c r="I12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" t="s">
+        <v>24</v>
+      </c>
+      <c r="K12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>208</v>
+      </c>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="I13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" t="s">
+        <v>24</v>
+      </c>
+      <c r="K13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>198</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14">
+        <v>626</v>
+      </c>
+      <c r="I14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>201</v>
+      </c>
+      <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15">
+        <v>62</v>
+      </c>
+      <c r="F15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" t="s">
+        <v>24</v>
+      </c>
+      <c r="K15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>205</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16">
+        <v>871</v>
+      </c>
+      <c r="I16" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16" t="s">
+        <v>24</v>
+      </c>
+      <c r="K16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>212</v>
+      </c>
+      <c r="B17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17">
+        <v>60</v>
+      </c>
+      <c r="I17" t="s">
+        <v>26</v>
+      </c>
+      <c r="J17" t="s">
+        <v>22</v>
+      </c>
+      <c r="K17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>213</v>
+      </c>
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18">
+        <v>65</v>
+      </c>
+      <c r="I18" t="s">
+        <v>26</v>
+      </c>
+      <c r="J18" t="s">
+        <v>22</v>
+      </c>
+      <c r="K18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <f>SUM(D9:D18)</f>
+        <v>2152</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>197</v>
+      </c>
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21">
+        <v>180</v>
+      </c>
+      <c r="E21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" t="s">
+        <v>14</v>
+      </c>
+      <c r="J21" t="s">
+        <v>24</v>
+      </c>
+      <c r="K21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>199</v>
+      </c>
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22">
+        <v>80</v>
+      </c>
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I22" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" t="s">
+        <v>24</v>
+      </c>
+      <c r="K22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>204</v>
+      </c>
+      <c r="B23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23">
+        <v>129</v>
+      </c>
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" t="s">
+        <v>13</v>
+      </c>
+      <c r="I23" t="s">
+        <v>14</v>
+      </c>
+      <c r="J23" t="s">
+        <v>24</v>
+      </c>
+      <c r="K23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>206</v>
+      </c>
+      <c r="B24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24">
+        <v>103</v>
+      </c>
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" t="s">
+        <v>18</v>
+      </c>
+      <c r="I24" t="s">
+        <v>14</v>
+      </c>
+      <c r="J24" t="s">
+        <v>24</v>
+      </c>
+      <c r="K24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>211</v>
+      </c>
+      <c r="B25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25">
+        <v>44</v>
+      </c>
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" t="s">
+        <v>13</v>
+      </c>
+      <c r="I25" t="s">
+        <v>14</v>
+      </c>
+      <c r="J25" t="s">
+        <v>24</v>
+      </c>
+      <c r="K25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>217</v>
+      </c>
+      <c r="B26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26">
+        <v>295</v>
+      </c>
+      <c r="E26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26" t="s">
+        <v>13</v>
+      </c>
+      <c r="I26" t="s">
+        <v>14</v>
+      </c>
+      <c r="J26" t="s">
+        <v>24</v>
+      </c>
+      <c r="K26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>229</v>
+      </c>
+      <c r="B27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27">
+        <v>191</v>
+      </c>
+      <c r="E27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" t="s">
+        <v>13</v>
+      </c>
+      <c r="I27" t="s">
+        <v>14</v>
+      </c>
+      <c r="J27" t="s">
+        <v>24</v>
+      </c>
+      <c r="K27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>230</v>
+      </c>
+      <c r="B28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28">
+        <v>90</v>
+      </c>
+      <c r="E28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" t="s">
+        <v>11</v>
+      </c>
+      <c r="H28" t="s">
+        <v>13</v>
+      </c>
+      <c r="I28" t="s">
+        <v>26</v>
+      </c>
+      <c r="J28" t="s">
+        <v>22</v>
+      </c>
+      <c r="K28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>220</v>
+      </c>
+      <c r="B29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29">
+        <v>278</v>
+      </c>
+      <c r="E29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" t="s">
+        <v>11</v>
+      </c>
+      <c r="H29" t="s">
+        <v>13</v>
+      </c>
+      <c r="I29" t="s">
+        <v>26</v>
+      </c>
+      <c r="J29" t="s">
+        <v>22</v>
+      </c>
+      <c r="K29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>214</v>
+      </c>
+      <c r="B30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30">
+        <v>16</v>
+      </c>
+      <c r="E30" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" t="s">
+        <v>13</v>
+      </c>
+      <c r="I30" t="s">
+        <v>26</v>
+      </c>
+      <c r="J30" t="s">
+        <v>22</v>
+      </c>
+      <c r="K30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>196</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" s="1">
+        <v>79</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>225</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="1">
+        <v>739</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>226</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" s="1">
+        <v>52</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>219</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D36" s="1">
+        <v>65</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>216</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37" s="1">
+        <v>119</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>209</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D38" s="1">
+        <v>38</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>202</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" s="1">
+        <v>42</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>203</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D40" s="1">
+        <v>76</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>227</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" s="1">
+        <v>379</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>228</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D42" s="1">
+        <v>45</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>210</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D43" s="1">
+        <v>47</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Bug fixes for augmentation. Resampling worker. Better MCMC implementation
</commit_message>
<xml_diff>
--- a/data/GroupSpec_cubic.xlsx
+++ b/data/GroupSpec_cubic.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DWMoreau/MLI/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A75EF3-81C1-5249-93AA-076E11C33163}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3649064D-0DA1-D74F-B794-F85BB93DA640}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5540" yWindow="880" windowWidth="24700" windowHeight="16840" xr2:uid="{7928E02C-29DC-574B-8667-D82DDE3DF551}"/>
+    <workbookView xWindow="1580" yWindow="-18660" windowWidth="26400" windowHeight="16940" activeTab="2" xr2:uid="{7EAE6936-6BB2-3145-B92E-F9D1A0613935}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
     <sheet name="Groups V0" sheetId="5" r:id="rId2"/>
     <sheet name="Groups V1" sheetId="7" r:id="rId3"/>
-    <sheet name="Groups V2" sheetId="6" r:id="rId4"/>
-    <sheet name="Groups V3" sheetId="8" r:id="rId5"/>
+    <sheet name="Groups V2" sheetId="9" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1288" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="71">
   <si>
     <t>spacegroup number</t>
   </si>
@@ -239,6 +238,9 @@
   </si>
   <si>
     <t>cubic_04</t>
+  </si>
+  <si>
+    <t>cubic_05</t>
   </si>
 </sst>
 </file>
@@ -600,9 +602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23E9EF93-9C26-5E4D-979F-BFF17FE810E6}">
   <dimension ref="A1:K168"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -660,7 +660,7 @@
         <v>63</v>
       </c>
       <c r="D2">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -674,7 +674,7 @@
         <v>63</v>
       </c>
       <c r="D3">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="E3" t="s">
         <v>64</v>
@@ -709,7 +709,7 @@
         <v>63</v>
       </c>
       <c r="D4">
-        <v>180</v>
+        <v>202</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -744,7 +744,8 @@
         <v>63</v>
       </c>
       <c r="D5">
-        <v>626</v>
+        <f>494 +  239</f>
+        <v>733</v>
       </c>
       <c r="I5" t="s">
         <v>14</v>
@@ -767,7 +768,7 @@
         <v>63</v>
       </c>
       <c r="D6">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -802,7 +803,7 @@
         <v>63</v>
       </c>
       <c r="D7">
-        <v>43</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -816,7 +817,7 @@
         <v>63</v>
       </c>
       <c r="D8">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="F8" t="s">
         <v>12</v>
@@ -848,7 +849,7 @@
         <v>63</v>
       </c>
       <c r="D9">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="E9" t="s">
         <v>64</v>
@@ -883,7 +884,7 @@
         <v>63</v>
       </c>
       <c r="D10">
-        <v>76</v>
+        <v>130</v>
       </c>
       <c r="E10" t="s">
         <v>64</v>
@@ -918,7 +919,7 @@
         <v>63</v>
       </c>
       <c r="D11">
-        <v>129</v>
+        <v>255</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -953,7 +954,8 @@
         <v>63</v>
       </c>
       <c r="D12">
-        <v>871</v>
+        <f>719 + 223</f>
+        <v>942</v>
       </c>
       <c r="I12" t="s">
         <v>14</v>
@@ -976,7 +978,7 @@
         <v>63</v>
       </c>
       <c r="D13">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -1011,7 +1013,7 @@
         <v>63</v>
       </c>
       <c r="D14">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -1025,7 +1027,7 @@
         <v>63</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="I15" t="s">
         <v>14</v>
@@ -1048,7 +1050,7 @@
         <v>63</v>
       </c>
       <c r="D16">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="E16" t="s">
         <v>64</v>
@@ -1083,7 +1085,7 @@
         <v>63</v>
       </c>
       <c r="D17">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E17" t="s">
         <v>64</v>
@@ -1118,7 +1120,7 @@
         <v>63</v>
       </c>
       <c r="D18">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -1153,7 +1155,7 @@
         <v>63</v>
       </c>
       <c r="D19">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="I19" t="s">
         <v>26</v>
@@ -1176,7 +1178,7 @@
         <v>63</v>
       </c>
       <c r="D20">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="I20" t="s">
         <v>26</v>
@@ -1199,7 +1201,7 @@
         <v>63</v>
       </c>
       <c r="D21">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E21" t="s">
         <v>10</v>
@@ -1234,7 +1236,8 @@
         <v>63</v>
       </c>
       <c r="D22">
-        <v>94</v>
+        <f>54 + 88</f>
+        <v>142</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -1248,7 +1251,8 @@
         <v>63</v>
       </c>
       <c r="D23">
-        <v>119</v>
+        <f>28 + 358</f>
+        <v>386</v>
       </c>
       <c r="E23" t="s">
         <v>64</v>
@@ -1283,7 +1287,8 @@
         <v>63</v>
       </c>
       <c r="D24">
-        <v>295</v>
+        <f>235 + 168</f>
+        <v>403</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
@@ -1318,7 +1323,8 @@
         <v>63</v>
       </c>
       <c r="D25">
-        <v>171</v>
+        <f>145 + 81</f>
+        <v>226</v>
       </c>
       <c r="I25" t="s">
         <v>14</v>
@@ -1341,7 +1347,7 @@
         <v>63</v>
       </c>
       <c r="D26">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="E26" t="s">
         <v>64</v>
@@ -1376,7 +1382,7 @@
         <v>63</v>
       </c>
       <c r="D27">
-        <v>278</v>
+        <v>440</v>
       </c>
       <c r="E27" t="s">
         <v>10</v>
@@ -1411,7 +1417,8 @@
         <v>63</v>
       </c>
       <c r="D28">
-        <v>483</v>
+        <f>228 + 955</f>
+        <v>1183</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
@@ -1425,7 +1432,8 @@
         <v>63</v>
       </c>
       <c r="D29">
-        <v>141</v>
+        <f>150</f>
+        <v>150</v>
       </c>
       <c r="F29" t="s">
         <v>12</v>
@@ -1457,7 +1465,8 @@
         <v>63</v>
       </c>
       <c r="D30">
-        <v>115</v>
+        <f>254 + 61</f>
+        <v>315</v>
       </c>
       <c r="I30" t="s">
         <v>14</v>
@@ -1480,7 +1489,7 @@
         <v>63</v>
       </c>
       <c r="D31">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="F31" t="s">
         <v>12</v>
@@ -1512,7 +1521,7 @@
         <v>63</v>
       </c>
       <c r="D32">
-        <v>739</v>
+        <v>1975</v>
       </c>
       <c r="E32" t="s">
         <v>64</v>
@@ -1547,7 +1556,7 @@
         <v>63</v>
       </c>
       <c r="D33">
-        <v>52</v>
+        <v>109</v>
       </c>
       <c r="E33" t="s">
         <v>64</v>
@@ -1582,7 +1591,8 @@
         <v>63</v>
       </c>
       <c r="D34">
-        <v>379</v>
+        <f>98 + 936</f>
+        <v>1034</v>
       </c>
       <c r="E34" t="s">
         <v>64</v>
@@ -1617,7 +1627,7 @@
         <v>63</v>
       </c>
       <c r="D35">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="E35" t="s">
         <v>64</v>
@@ -1652,7 +1662,8 @@
         <v>63</v>
       </c>
       <c r="D36">
-        <v>191</v>
+        <f>107 + 282</f>
+        <v>389</v>
       </c>
       <c r="E36" t="s">
         <v>10</v>
@@ -1687,7 +1698,7 @@
         <v>63</v>
       </c>
       <c r="D37">
-        <v>90</v>
+        <v>222</v>
       </c>
       <c r="E37" t="s">
         <v>10</v>
@@ -1742,11 +1753,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC97E7B2-CD49-3E49-A19E-E59CA308682C}">
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:K168"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -1796,7 +1805,7 @@
         <v>65</v>
       </c>
       <c r="D2">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -1810,7 +1819,7 @@
         <v>65</v>
       </c>
       <c r="D3">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="E3" t="s">
         <v>64</v>
@@ -1845,7 +1854,7 @@
         <v>65</v>
       </c>
       <c r="D4">
-        <v>180</v>
+        <v>202</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -1880,7 +1889,8 @@
         <v>65</v>
       </c>
       <c r="D5">
-        <v>626</v>
+        <f>494 +  239</f>
+        <v>733</v>
       </c>
       <c r="I5" t="s">
         <v>14</v>
@@ -1903,7 +1913,7 @@
         <v>65</v>
       </c>
       <c r="D6">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -1938,7 +1948,7 @@
         <v>65</v>
       </c>
       <c r="D7">
-        <v>43</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -1952,7 +1962,7 @@
         <v>65</v>
       </c>
       <c r="D8">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="F8" t="s">
         <v>12</v>
@@ -1984,7 +1994,7 @@
         <v>65</v>
       </c>
       <c r="D9">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="E9" t="s">
         <v>64</v>
@@ -2019,7 +2029,7 @@
         <v>65</v>
       </c>
       <c r="D10">
-        <v>76</v>
+        <v>130</v>
       </c>
       <c r="E10" t="s">
         <v>64</v>
@@ -2054,7 +2064,7 @@
         <v>65</v>
       </c>
       <c r="D11">
-        <v>129</v>
+        <v>255</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -2089,7 +2099,8 @@
         <v>65</v>
       </c>
       <c r="D12">
-        <v>871</v>
+        <f>719 + 223</f>
+        <v>942</v>
       </c>
       <c r="I12" t="s">
         <v>14</v>
@@ -2112,7 +2123,7 @@
         <v>65</v>
       </c>
       <c r="D13">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -2147,7 +2158,7 @@
         <v>65</v>
       </c>
       <c r="D14">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -2161,7 +2172,7 @@
         <v>65</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="I15" t="s">
         <v>14</v>
@@ -2184,7 +2195,7 @@
         <v>65</v>
       </c>
       <c r="D16">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="E16" t="s">
         <v>64</v>
@@ -2219,7 +2230,7 @@
         <v>65</v>
       </c>
       <c r="D17">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E17" t="s">
         <v>64</v>
@@ -2254,7 +2265,7 @@
         <v>65</v>
       </c>
       <c r="D18">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -2289,7 +2300,7 @@
         <v>65</v>
       </c>
       <c r="D19">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="I19" t="s">
         <v>26</v>
@@ -2312,7 +2323,7 @@
         <v>65</v>
       </c>
       <c r="D20">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="I20" t="s">
         <v>26</v>
@@ -2335,7 +2346,7 @@
         <v>65</v>
       </c>
       <c r="D21">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E21" t="s">
         <v>10</v>
@@ -2370,7 +2381,8 @@
         <v>65</v>
       </c>
       <c r="D22">
-        <v>94</v>
+        <f>54 + 88</f>
+        <v>142</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -2384,7 +2396,8 @@
         <v>65</v>
       </c>
       <c r="D23">
-        <v>119</v>
+        <f>28 + 358</f>
+        <v>386</v>
       </c>
       <c r="E23" t="s">
         <v>64</v>
@@ -2419,7 +2432,8 @@
         <v>65</v>
       </c>
       <c r="D24">
-        <v>295</v>
+        <f>235 + 168</f>
+        <v>403</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
@@ -2454,7 +2468,8 @@
         <v>65</v>
       </c>
       <c r="D25">
-        <v>171</v>
+        <f>145 + 81</f>
+        <v>226</v>
       </c>
       <c r="I25" t="s">
         <v>14</v>
@@ -2477,7 +2492,7 @@
         <v>65</v>
       </c>
       <c r="D26">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="E26" t="s">
         <v>64</v>
@@ -2512,7 +2527,7 @@
         <v>65</v>
       </c>
       <c r="D27">
-        <v>278</v>
+        <v>440</v>
       </c>
       <c r="E27" t="s">
         <v>10</v>
@@ -2547,7 +2562,8 @@
         <v>65</v>
       </c>
       <c r="D28">
-        <v>483</v>
+        <f>228 + 955</f>
+        <v>1183</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
@@ -2561,7 +2577,8 @@
         <v>65</v>
       </c>
       <c r="D29">
-        <v>141</v>
+        <f>150</f>
+        <v>150</v>
       </c>
       <c r="F29" t="s">
         <v>12</v>
@@ -2593,7 +2610,8 @@
         <v>65</v>
       </c>
       <c r="D30">
-        <v>115</v>
+        <f>254 + 61</f>
+        <v>315</v>
       </c>
       <c r="I30" t="s">
         <v>14</v>
@@ -2616,7 +2634,7 @@
         <v>65</v>
       </c>
       <c r="D31">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="F31" t="s">
         <v>12</v>
@@ -2648,7 +2666,7 @@
         <v>65</v>
       </c>
       <c r="D32">
-        <v>739</v>
+        <v>1975</v>
       </c>
       <c r="E32" t="s">
         <v>64</v>
@@ -2683,7 +2701,7 @@
         <v>65</v>
       </c>
       <c r="D33">
-        <v>52</v>
+        <v>109</v>
       </c>
       <c r="E33" t="s">
         <v>64</v>
@@ -2718,7 +2736,8 @@
         <v>65</v>
       </c>
       <c r="D34">
-        <v>379</v>
+        <f>98 + 936</f>
+        <v>1034</v>
       </c>
       <c r="E34" t="s">
         <v>64</v>
@@ -2753,7 +2772,7 @@
         <v>65</v>
       </c>
       <c r="D35">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="E35" t="s">
         <v>64</v>
@@ -2788,7 +2807,8 @@
         <v>65</v>
       </c>
       <c r="D36">
-        <v>191</v>
+        <f>107 + 282</f>
+        <v>389</v>
       </c>
       <c r="E36" t="s">
         <v>10</v>
@@ -2823,7 +2843,7 @@
         <v>65</v>
       </c>
       <c r="D37">
-        <v>90</v>
+        <v>222</v>
       </c>
       <c r="E37" t="s">
         <v>10</v>
@@ -2846,6 +2866,24 @@
       <c r="K37" t="s">
         <v>23</v>
       </c>
+    </row>
+    <row r="147" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D147" s="1"/>
+    </row>
+    <row r="148" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D148" s="1"/>
+    </row>
+    <row r="153" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D153" s="1"/>
+    </row>
+    <row r="159" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D159" s="1"/>
+    </row>
+    <row r="160" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D160" s="1"/>
+    </row>
+    <row r="168" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D168" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2856,8 +2894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A60AFE1-6AB8-D64E-9454-61131BC5B2BC}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2911,7 +2949,7 @@
         <v>65</v>
       </c>
       <c r="D2">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -2925,7 +2963,7 @@
         <v>65</v>
       </c>
       <c r="D3">
-        <v>626</v>
+        <v>733</v>
       </c>
       <c r="I3" t="s">
         <v>14</v>
@@ -2948,7 +2986,7 @@
         <v>65</v>
       </c>
       <c r="D4">
-        <v>43</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -2962,7 +3000,7 @@
         <v>65</v>
       </c>
       <c r="D5">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="F5" t="s">
         <v>12</v>
@@ -2994,7 +3032,8 @@
         <v>65</v>
       </c>
       <c r="D6">
-        <v>871</v>
+        <f>719 + 223</f>
+        <v>942</v>
       </c>
       <c r="I6" t="s">
         <v>14</v>
@@ -3017,7 +3056,7 @@
         <v>65</v>
       </c>
       <c r="D7">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -3031,7 +3070,7 @@
         <v>65</v>
       </c>
       <c r="D8">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="I8" t="s">
         <v>14</v>
@@ -3053,8 +3092,8 @@
       <c r="C9" t="s">
         <v>65</v>
       </c>
-      <c r="D9">
-        <v>60</v>
+      <c r="D9" s="1">
+        <v>80</v>
       </c>
       <c r="I9" t="s">
         <v>26</v>
@@ -3076,8 +3115,8 @@
       <c r="C10" t="s">
         <v>65</v>
       </c>
-      <c r="D10">
-        <v>65</v>
+      <c r="D10" s="1">
+        <v>90</v>
       </c>
       <c r="I10" t="s">
         <v>26</v>
@@ -3100,7 +3139,8 @@
         <v>65</v>
       </c>
       <c r="D11">
-        <v>94</v>
+        <f>54 + 88</f>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -3114,7 +3154,8 @@
         <v>65</v>
       </c>
       <c r="D12">
-        <v>171</v>
+        <f>145 + 81</f>
+        <v>226</v>
       </c>
       <c r="I12" t="s">
         <v>14</v>
@@ -3137,7 +3178,8 @@
         <v>65</v>
       </c>
       <c r="D13">
-        <v>483</v>
+        <f>228 + 955</f>
+        <v>1183</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -3151,7 +3193,8 @@
         <v>65</v>
       </c>
       <c r="D14">
-        <v>141</v>
+        <f>150</f>
+        <v>150</v>
       </c>
       <c r="F14" t="s">
         <v>12</v>
@@ -3183,7 +3226,8 @@
         <v>65</v>
       </c>
       <c r="D15">
-        <v>115</v>
+        <f>254 + 61</f>
+        <v>315</v>
       </c>
       <c r="I15" t="s">
         <v>14</v>
@@ -3206,7 +3250,7 @@
         <v>65</v>
       </c>
       <c r="D16">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="F16" t="s">
         <v>12</v>
@@ -3230,7 +3274,7 @@
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D17">
         <f>SUM(D2:D16)</f>
-        <v>2820</v>
+        <v>4165</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -3244,7 +3288,7 @@
         <v>66</v>
       </c>
       <c r="D19">
-        <v>180</v>
+        <v>202</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -3279,7 +3323,7 @@
         <v>66</v>
       </c>
       <c r="D20">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -3314,7 +3358,7 @@
         <v>66</v>
       </c>
       <c r="D21">
-        <v>129</v>
+        <v>255</v>
       </c>
       <c r="E21" t="s">
         <v>10</v>
@@ -3349,7 +3393,7 @@
         <v>66</v>
       </c>
       <c r="D22">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="E22" t="s">
         <v>10</v>
@@ -3384,7 +3428,7 @@
         <v>66</v>
       </c>
       <c r="D23">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="E23" t="s">
         <v>10</v>
@@ -3419,7 +3463,7 @@
         <v>66</v>
       </c>
       <c r="D24">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
@@ -3454,7 +3498,8 @@
         <v>66</v>
       </c>
       <c r="D25">
-        <v>295</v>
+        <f>235 + 168</f>
+        <v>403</v>
       </c>
       <c r="E25" t="s">
         <v>10</v>
@@ -3489,7 +3534,7 @@
         <v>66</v>
       </c>
       <c r="D26">
-        <v>278</v>
+        <v>440</v>
       </c>
       <c r="E26" t="s">
         <v>10</v>
@@ -3524,7 +3569,8 @@
         <v>66</v>
       </c>
       <c r="D27">
-        <v>191</v>
+        <f>107 + 282</f>
+        <v>389</v>
       </c>
       <c r="E27" t="s">
         <v>10</v>
@@ -3559,7 +3605,7 @@
         <v>66</v>
       </c>
       <c r="D28">
-        <v>90</v>
+        <v>222</v>
       </c>
       <c r="E28" t="s">
         <v>10</v>
@@ -3586,7 +3632,7 @@
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D29">
         <f>SUM(D19:D28)</f>
-        <v>1406</v>
+        <v>2222</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
@@ -3600,7 +3646,7 @@
         <v>67</v>
       </c>
       <c r="D31">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="E31" t="s">
         <v>64</v>
@@ -3635,7 +3681,7 @@
         <v>67</v>
       </c>
       <c r="D32">
-        <v>739</v>
+        <v>1975</v>
       </c>
       <c r="E32" t="s">
         <v>64</v>
@@ -3670,7 +3716,7 @@
         <v>67</v>
       </c>
       <c r="D33">
-        <v>52</v>
+        <v>109</v>
       </c>
       <c r="E33" t="s">
         <v>64</v>
@@ -3705,7 +3751,8 @@
         <v>67</v>
       </c>
       <c r="D34">
-        <v>379</v>
+        <f>98 + 936</f>
+        <v>1034</v>
       </c>
       <c r="E34" t="s">
         <v>64</v>
@@ -3740,7 +3787,7 @@
         <v>67</v>
       </c>
       <c r="D35">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="E35" t="s">
         <v>64</v>
@@ -3775,7 +3822,7 @@
         <v>67</v>
       </c>
       <c r="D36">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="E36" t="s">
         <v>64</v>
@@ -3810,7 +3857,8 @@
         <v>67</v>
       </c>
       <c r="D37">
-        <v>119</v>
+        <f>28 + 358</f>
+        <v>386</v>
       </c>
       <c r="E37" t="s">
         <v>64</v>
@@ -3845,7 +3893,7 @@
         <v>67</v>
       </c>
       <c r="D38">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="E38" t="s">
         <v>64</v>
@@ -3880,7 +3928,7 @@
         <v>67</v>
       </c>
       <c r="D39">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E39" t="s">
         <v>64</v>
@@ -3915,7 +3963,7 @@
         <v>67</v>
       </c>
       <c r="D40">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="E40" t="s">
         <v>64</v>
@@ -3950,7 +3998,7 @@
         <v>67</v>
       </c>
       <c r="D41">
-        <v>76</v>
+        <v>130</v>
       </c>
       <c r="E41" t="s">
         <v>64</v>
@@ -3977,7 +4025,7 @@
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D42">
         <f>SUM(D31:D41)</f>
-        <v>1681</v>
+        <v>3980</v>
       </c>
     </row>
   </sheetData>
@@ -3986,18 +4034,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFC2BFA0-9478-3A49-B32B-95904FA22C6D}">
-  <dimension ref="A1:K46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9938544-366F-104B-B48D-929943AE788E}">
+  <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C45" sqref="C45:C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="5" max="5" width="28" customWidth="1"/>
-    <col min="6" max="8" width="18.33203125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -4045,7 +4089,7 @@
         <v>65</v>
       </c>
       <c r="D2">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -4059,7 +4103,7 @@
         <v>65</v>
       </c>
       <c r="D3">
-        <v>43</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -4073,7 +4117,7 @@
         <v>65</v>
       </c>
       <c r="D4">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -4087,7 +4131,8 @@
         <v>65</v>
       </c>
       <c r="D5">
-        <v>94</v>
+        <f>54 + 88</f>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -4101,50 +4146,43 @@
         <v>65</v>
       </c>
       <c r="D6">
-        <v>483</v>
+        <f>228 + 955</f>
+        <v>1183</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>215</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" t="s">
+        <v>65</v>
+      </c>
       <c r="D7">
-        <f>SUM(D2:D6)</f>
-        <v>668</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>201</v>
-      </c>
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" t="s">
-        <v>66</v>
-      </c>
-      <c r="D9">
-        <v>62</v>
-      </c>
-      <c r="I9" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" t="s">
-        <v>24</v>
-      </c>
-      <c r="K9" t="s">
-        <v>15</v>
+        <f>54 + 88</f>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <f>SUM(D2:D7)</f>
+        <v>1599</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
         <v>66</v>
       </c>
       <c r="D10">
-        <v>129</v>
+        <v>733</v>
       </c>
       <c r="I10" t="s">
         <v>14</v>
@@ -4158,16 +4196,25 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
         <v>66</v>
       </c>
       <c r="D11">
-        <v>871</v>
+        <v>106</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" t="s">
+        <v>13</v>
       </c>
       <c r="I11" t="s">
         <v>14</v>
@@ -4181,16 +4228,17 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
         <v>66</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <f>719 + 223</f>
+        <v>942</v>
       </c>
       <c r="I12" t="s">
         <v>14</v>
@@ -4204,16 +4252,16 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
         <v>66</v>
       </c>
       <c r="D13">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="I13" t="s">
         <v>14</v>
@@ -4227,16 +4275,17 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
         <v>66</v>
       </c>
       <c r="D14">
-        <v>295</v>
+        <f>145 + 81</f>
+        <v>226</v>
       </c>
       <c r="I14" t="s">
         <v>14</v>
@@ -4250,16 +4299,26 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C15" t="s">
         <v>66</v>
       </c>
       <c r="D15">
-        <v>171</v>
+        <f>150</f>
+        <v>150</v>
+      </c>
+      <c r="F15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" t="s">
+        <v>13</v>
       </c>
       <c r="I15" t="s">
         <v>14</v>
@@ -4273,16 +4332,17 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C16" t="s">
         <v>66</v>
       </c>
       <c r="D16">
-        <v>141</v>
+        <f>254 + 61</f>
+        <v>315</v>
       </c>
       <c r="I16" t="s">
         <v>14</v>
@@ -4296,16 +4356,25 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s">
         <v>66</v>
       </c>
       <c r="D17">
-        <v>115</v>
+        <v>57</v>
+      </c>
+      <c r="F17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" t="s">
+        <v>13</v>
       </c>
       <c r="I17" t="s">
         <v>14</v>
@@ -4319,137 +4388,176 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C18" t="s">
         <v>66</v>
       </c>
-      <c r="D18">
-        <v>38</v>
+      <c r="D18" s="1">
+        <v>80</v>
       </c>
       <c r="I18" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="J18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="K18" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="C19" t="s">
         <v>66</v>
       </c>
-      <c r="D19">
-        <v>191</v>
+      <c r="D19" s="1">
+        <v>90</v>
       </c>
       <c r="I19" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="J19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="K19" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>197</v>
-      </c>
-      <c r="B20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" t="s">
-        <v>66</v>
-      </c>
       <c r="D20">
-        <v>180</v>
-      </c>
-      <c r="I20" t="s">
-        <v>14</v>
-      </c>
-      <c r="J20" t="s">
-        <v>24</v>
-      </c>
-      <c r="K20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>198</v>
-      </c>
-      <c r="B21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" t="s">
-        <v>66</v>
-      </c>
-      <c r="D21">
-        <v>626</v>
-      </c>
-      <c r="I21" t="s">
-        <v>14</v>
-      </c>
-      <c r="J21" t="s">
-        <v>24</v>
-      </c>
-      <c r="K21" t="s">
-        <v>15</v>
+        <f>SUM(D10:D19)</f>
+        <v>2708</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
+        <v>197</v>
+      </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22">
+        <v>202</v>
+      </c>
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I22" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" t="s">
+        <v>24</v>
+      </c>
+      <c r="K22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23">
         <v>199</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>31</v>
       </c>
-      <c r="C22" t="s">
-        <v>66</v>
-      </c>
-      <c r="D22">
-        <v>80</v>
-      </c>
-      <c r="I22" t="s">
-        <v>14</v>
-      </c>
-      <c r="J22" t="s">
-        <v>24</v>
-      </c>
-      <c r="K22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>67</v>
+      </c>
       <c r="D23">
-        <f>SUM(D9:D22)</f>
-        <v>2946</v>
+        <v>100</v>
+      </c>
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" t="s">
+        <v>13</v>
+      </c>
+      <c r="I23" t="s">
+        <v>14</v>
+      </c>
+      <c r="J23" t="s">
+        <v>24</v>
+      </c>
+      <c r="K23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>204</v>
+      </c>
+      <c r="B24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24">
+        <v>255</v>
+      </c>
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" t="s">
+        <v>11</v>
+      </c>
+      <c r="H24" t="s">
+        <v>13</v>
+      </c>
+      <c r="I24" t="s">
+        <v>14</v>
+      </c>
+      <c r="J24" t="s">
+        <v>24</v>
+      </c>
+      <c r="K24" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C25" t="s">
         <v>67</v>
       </c>
       <c r="D25">
-        <v>42</v>
+        <v>128</v>
+      </c>
+      <c r="E25" t="s">
+        <v>10</v>
       </c>
       <c r="F25" t="s">
         <v>16</v>
@@ -4472,25 +4580,28 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C26" t="s">
         <v>67</v>
       </c>
       <c r="D26">
-        <v>103</v>
+        <v>57</v>
+      </c>
+      <c r="E26" t="s">
+        <v>10</v>
       </c>
       <c r="F26" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G26" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="H26" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="I26" t="s">
         <v>14</v>
@@ -4504,25 +4615,29 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="B27" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C27" t="s">
         <v>67</v>
       </c>
       <c r="D27">
-        <v>38</v>
+        <f>235 + 168</f>
+        <v>403</v>
+      </c>
+      <c r="E27" t="s">
+        <v>10</v>
       </c>
       <c r="F27" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G27" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="H27" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="I27" t="s">
         <v>14</v>
@@ -4536,25 +4651,29 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>216</v>
+        <v>229</v>
       </c>
       <c r="B28" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="C28" t="s">
         <v>67</v>
       </c>
       <c r="D28">
-        <v>119</v>
+        <f>107 + 282</f>
+        <v>389</v>
+      </c>
+      <c r="E28" t="s">
+        <v>10</v>
       </c>
       <c r="F28" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G28" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="H28" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="I28" t="s">
         <v>14</v>
@@ -4567,272 +4686,348 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>219</v>
-      </c>
-      <c r="B29" t="s">
-        <v>51</v>
-      </c>
-      <c r="C29" t="s">
-        <v>67</v>
-      </c>
       <c r="D29">
-        <v>65</v>
-      </c>
-      <c r="F29" t="s">
-        <v>16</v>
-      </c>
-      <c r="G29" t="s">
-        <v>17</v>
-      </c>
-      <c r="H29" t="s">
-        <v>18</v>
-      </c>
-      <c r="I29" t="s">
-        <v>14</v>
-      </c>
-      <c r="J29" t="s">
-        <v>24</v>
-      </c>
-      <c r="K29" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>225</v>
-      </c>
-      <c r="B30" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30" t="s">
-        <v>67</v>
-      </c>
-      <c r="D30">
-        <v>739</v>
-      </c>
-      <c r="F30" t="s">
-        <v>16</v>
-      </c>
-      <c r="G30" t="s">
-        <v>17</v>
-      </c>
-      <c r="H30" t="s">
-        <v>18</v>
-      </c>
-      <c r="I30" t="s">
-        <v>14</v>
-      </c>
-      <c r="J30" t="s">
-        <v>24</v>
-      </c>
-      <c r="K30" t="s">
-        <v>15</v>
+        <f>SUM(D22:D28)</f>
+        <v>1534</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="B31" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C31" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D31">
-        <v>52</v>
+        <v>26</v>
+      </c>
+      <c r="E31" t="s">
+        <v>10</v>
       </c>
       <c r="F31" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G31" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="H31" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="I31" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="J31" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="K31" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>196</v>
+        <v>220</v>
       </c>
       <c r="B32" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="C32" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D32">
-        <v>79</v>
+        <v>440</v>
+      </c>
+      <c r="E32" t="s">
+        <v>10</v>
       </c>
       <c r="F32" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G32" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="H32" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="I32" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="J32" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="K32" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>230</v>
+      </c>
+      <c r="B33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" t="s">
+        <v>68</v>
+      </c>
       <c r="D33">
-        <f>SUM(D25:D32)</f>
-        <v>1237</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>220</v>
-      </c>
-      <c r="B35" t="s">
-        <v>52</v>
-      </c>
-      <c r="C35" t="s">
-        <v>68</v>
-      </c>
-      <c r="D35">
-        <v>278</v>
-      </c>
-      <c r="I35" t="s">
+        <v>222</v>
+      </c>
+      <c r="E33" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33" t="s">
+        <v>11</v>
+      </c>
+      <c r="H33" t="s">
+        <v>13</v>
+      </c>
+      <c r="I33" t="s">
         <v>26</v>
       </c>
-      <c r="J35" t="s">
+      <c r="J33" t="s">
         <v>22</v>
       </c>
-      <c r="K35" t="s">
+      <c r="K33" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D34">
+        <f>SUM(D31:D33)</f>
+        <v>688</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="B36" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C36" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D36">
-        <v>60</v>
+        <v>88</v>
+      </c>
+      <c r="E36" t="s">
+        <v>64</v>
+      </c>
+      <c r="F36" t="s">
+        <v>16</v>
+      </c>
+      <c r="G36" t="s">
+        <v>17</v>
+      </c>
+      <c r="H36" t="s">
+        <v>18</v>
       </c>
       <c r="I36" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="J36" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K36" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>213</v>
+        <v>225</v>
       </c>
       <c r="B37" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="C37" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D37">
-        <v>65</v>
+        <v>1975</v>
+      </c>
+      <c r="E37" t="s">
+        <v>64</v>
+      </c>
+      <c r="F37" t="s">
+        <v>16</v>
+      </c>
+      <c r="G37" t="s">
+        <v>17</v>
+      </c>
+      <c r="H37" t="s">
+        <v>18</v>
       </c>
       <c r="I37" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="J37" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K37" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="B38" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C38" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D38">
+        <v>109</v>
+      </c>
+      <c r="E38" t="s">
+        <v>64</v>
+      </c>
+      <c r="F38" t="s">
         <v>16</v>
       </c>
+      <c r="G38" t="s">
+        <v>17</v>
+      </c>
+      <c r="H38" t="s">
+        <v>18</v>
+      </c>
       <c r="I38" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="J38" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K38" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="B39" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C39" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D39">
-        <v>90</v>
+        <v>78</v>
+      </c>
+      <c r="E39" t="s">
+        <v>64</v>
+      </c>
+      <c r="F39" t="s">
+        <v>16</v>
+      </c>
+      <c r="G39" t="s">
+        <v>17</v>
+      </c>
+      <c r="H39" t="s">
+        <v>18</v>
       </c>
       <c r="I39" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="J39" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K39" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>216</v>
+      </c>
+      <c r="B40" t="s">
+        <v>48</v>
+      </c>
+      <c r="C40" t="s">
+        <v>69</v>
+      </c>
       <c r="D40">
-        <f>SUM(D35:D39)</f>
-        <v>509</v>
+        <f>28 + 358</f>
+        <v>386</v>
+      </c>
+      <c r="E40" t="s">
+        <v>64</v>
+      </c>
+      <c r="F40" t="s">
+        <v>16</v>
+      </c>
+      <c r="G40" t="s">
+        <v>17</v>
+      </c>
+      <c r="H40" t="s">
+        <v>18</v>
+      </c>
+      <c r="I40" t="s">
+        <v>14</v>
+      </c>
+      <c r="J40" t="s">
+        <v>24</v>
+      </c>
+      <c r="K40" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>209</v>
+      </c>
+      <c r="B41" t="s">
+        <v>41</v>
+      </c>
+      <c r="C41" t="s">
+        <v>69</v>
+      </c>
+      <c r="D41">
+        <v>43</v>
+      </c>
+      <c r="E41" t="s">
+        <v>64</v>
+      </c>
+      <c r="F41" t="s">
+        <v>16</v>
+      </c>
+      <c r="G41" t="s">
+        <v>17</v>
+      </c>
+      <c r="H41" t="s">
+        <v>18</v>
+      </c>
+      <c r="I41" t="s">
+        <v>14</v>
+      </c>
+      <c r="J41" t="s">
+        <v>24</v>
+      </c>
+      <c r="K41" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B42" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C42" t="s">
         <v>69</v>
       </c>
       <c r="D42">
-        <v>47</v>
+        <v>68</v>
+      </c>
+      <c r="E42" t="s">
+        <v>64</v>
       </c>
       <c r="F42" t="s">
         <v>16</v>
@@ -4844,77 +5039,19 @@
         <v>18</v>
       </c>
       <c r="I42" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="J42" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K42" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>227</v>
-      </c>
-      <c r="B43" t="s">
-        <v>59</v>
-      </c>
-      <c r="C43" t="s">
-        <v>69</v>
-      </c>
       <c r="D43">
-        <v>379</v>
-      </c>
-      <c r="F43" t="s">
-        <v>16</v>
-      </c>
-      <c r="G43" t="s">
-        <v>17</v>
-      </c>
-      <c r="H43" t="s">
-        <v>18</v>
-      </c>
-      <c r="I43" t="s">
-        <v>26</v>
-      </c>
-      <c r="J43" t="s">
-        <v>22</v>
-      </c>
-      <c r="K43" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>228</v>
-      </c>
-      <c r="B44" t="s">
-        <v>60</v>
-      </c>
-      <c r="C44" t="s">
-        <v>69</v>
-      </c>
-      <c r="D44">
-        <v>45</v>
-      </c>
-      <c r="F44" t="s">
-        <v>16</v>
-      </c>
-      <c r="G44" t="s">
-        <v>17</v>
-      </c>
-      <c r="H44" t="s">
-        <v>18</v>
-      </c>
-      <c r="I44" t="s">
-        <v>26</v>
-      </c>
-      <c r="J44" t="s">
-        <v>22</v>
-      </c>
-      <c r="K44" t="s">
-        <v>23</v>
+        <f>SUM(D36:D42)</f>
+        <v>2747</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
@@ -4925,19 +5062,22 @@
         <v>35</v>
       </c>
       <c r="C45" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D45">
-        <v>76</v>
+        <v>130</v>
+      </c>
+      <c r="E45" t="s">
+        <v>64</v>
       </c>
       <c r="F45" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G45" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H45" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I45" t="s">
         <v>26</v>
@@ -4950,1136 +5090,115 @@
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>227</v>
+      </c>
+      <c r="B46" t="s">
+        <v>59</v>
+      </c>
+      <c r="C46" t="s">
+        <v>70</v>
+      </c>
       <c r="D46">
-        <f>SUM(D42:D45)</f>
-        <v>547</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A97EA6C-E4EF-694D-8776-4A662F7FA16D}">
-  <dimension ref="A1:K43"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28:K30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="5" max="5" width="27.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>195</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D2">
+        <f>98 + 936</f>
+        <v>1034</v>
+      </c>
+      <c r="E46" t="s">
+        <v>64</v>
+      </c>
+      <c r="F46" t="s">
+        <v>20</v>
+      </c>
+      <c r="G46" t="s">
+        <v>21</v>
+      </c>
+      <c r="H46" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>200</v>
-      </c>
-      <c r="B3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3">
+      <c r="I46" t="s">
+        <v>26</v>
+      </c>
+      <c r="J46" t="s">
+        <v>22</v>
+      </c>
+      <c r="K46" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>228</v>
+      </c>
+      <c r="B47" t="s">
+        <v>60</v>
+      </c>
+      <c r="C47" t="s">
+        <v>70</v>
+      </c>
+      <c r="D47">
+        <v>26</v>
+      </c>
+      <c r="E47" t="s">
+        <v>64</v>
+      </c>
+      <c r="F47" t="s">
+        <v>20</v>
+      </c>
+      <c r="G47" t="s">
+        <v>21</v>
+      </c>
+      <c r="H47" t="s">
+        <v>19</v>
+      </c>
+      <c r="I47" t="s">
+        <v>26</v>
+      </c>
+      <c r="J47" t="s">
+        <v>22</v>
+      </c>
+      <c r="K47" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>210</v>
+      </c>
+      <c r="B48" t="s">
+        <v>42</v>
+      </c>
+      <c r="C48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D48">
         <v>43</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>207</v>
-      </c>
-      <c r="B4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D4">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>215</v>
-      </c>
-      <c r="B5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D5">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>221</v>
-      </c>
-      <c r="B6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D6">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D7">
-        <f>SUM(D2:D6)</f>
-        <v>668</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>222</v>
-      </c>
-      <c r="B9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" t="s">
-        <v>66</v>
-      </c>
-      <c r="D9">
-        <v>141</v>
-      </c>
-      <c r="F9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" t="s">
-        <v>24</v>
-      </c>
-      <c r="K9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>223</v>
-      </c>
-      <c r="B10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" t="s">
-        <v>66</v>
-      </c>
-      <c r="D10">
-        <v>115</v>
-      </c>
-      <c r="I10" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" t="s">
-        <v>24</v>
-      </c>
-      <c r="K10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>224</v>
-      </c>
-      <c r="B11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11">
-        <v>38</v>
-      </c>
-      <c r="F11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" t="s">
-        <v>13</v>
-      </c>
-      <c r="I11" t="s">
-        <v>14</v>
-      </c>
-      <c r="J11" t="s">
-        <v>24</v>
-      </c>
-      <c r="K11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>218</v>
-      </c>
-      <c r="B12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D12">
-        <v>171</v>
-      </c>
-      <c r="I12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J12" t="s">
-        <v>24</v>
-      </c>
-      <c r="K12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>208</v>
-      </c>
-      <c r="B13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" t="s">
-        <v>66</v>
-      </c>
-      <c r="D13">
-        <v>3</v>
-      </c>
-      <c r="I13" t="s">
-        <v>14</v>
-      </c>
-      <c r="J13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>198</v>
-      </c>
-      <c r="B14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14">
-        <v>626</v>
-      </c>
-      <c r="I14" t="s">
-        <v>14</v>
-      </c>
-      <c r="J14" t="s">
-        <v>24</v>
-      </c>
-      <c r="K14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>201</v>
-      </c>
-      <c r="B15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" t="s">
-        <v>66</v>
-      </c>
-      <c r="D15">
-        <v>62</v>
-      </c>
-      <c r="F15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I15" t="s">
-        <v>14</v>
-      </c>
-      <c r="J15" t="s">
-        <v>24</v>
-      </c>
-      <c r="K15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>205</v>
-      </c>
-      <c r="B16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" t="s">
-        <v>66</v>
-      </c>
-      <c r="D16">
-        <v>871</v>
-      </c>
-      <c r="I16" t="s">
-        <v>14</v>
-      </c>
-      <c r="J16" t="s">
-        <v>24</v>
-      </c>
-      <c r="K16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>212</v>
-      </c>
-      <c r="B17" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" t="s">
-        <v>66</v>
-      </c>
-      <c r="D17">
-        <v>60</v>
-      </c>
-      <c r="I17" t="s">
+      <c r="E48" t="s">
+        <v>64</v>
+      </c>
+      <c r="F48" t="s">
+        <v>16</v>
+      </c>
+      <c r="G48" t="s">
+        <v>17</v>
+      </c>
+      <c r="H48" t="s">
+        <v>18</v>
+      </c>
+      <c r="I48" t="s">
         <v>26</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J48" t="s">
         <v>22</v>
       </c>
-      <c r="K17" t="s">
+      <c r="K48" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>213</v>
-      </c>
-      <c r="B18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" t="s">
-        <v>66</v>
-      </c>
-      <c r="D18">
-        <v>65</v>
-      </c>
-      <c r="I18" t="s">
-        <v>26</v>
-      </c>
-      <c r="J18" t="s">
-        <v>22</v>
-      </c>
-      <c r="K18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D19">
-        <f>SUM(D9:D18)</f>
-        <v>2152</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>197</v>
-      </c>
-      <c r="B21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" t="s">
-        <v>67</v>
-      </c>
-      <c r="D21">
-        <v>180</v>
-      </c>
-      <c r="E21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" t="s">
-        <v>11</v>
-      </c>
-      <c r="H21" t="s">
-        <v>13</v>
-      </c>
-      <c r="I21" t="s">
-        <v>14</v>
-      </c>
-      <c r="J21" t="s">
-        <v>24</v>
-      </c>
-      <c r="K21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>199</v>
-      </c>
-      <c r="B22" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22" t="s">
-        <v>67</v>
-      </c>
-      <c r="D22">
-        <v>80</v>
-      </c>
-      <c r="E22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22" t="s">
-        <v>12</v>
-      </c>
-      <c r="G22" t="s">
-        <v>11</v>
-      </c>
-      <c r="H22" t="s">
-        <v>13</v>
-      </c>
-      <c r="I22" t="s">
-        <v>14</v>
-      </c>
-      <c r="J22" t="s">
-        <v>24</v>
-      </c>
-      <c r="K22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>204</v>
-      </c>
-      <c r="B23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" t="s">
-        <v>67</v>
-      </c>
-      <c r="D23">
-        <v>129</v>
-      </c>
-      <c r="E23" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" t="s">
-        <v>12</v>
-      </c>
-      <c r="G23" t="s">
-        <v>11</v>
-      </c>
-      <c r="H23" t="s">
-        <v>13</v>
-      </c>
-      <c r="I23" t="s">
-        <v>14</v>
-      </c>
-      <c r="J23" t="s">
-        <v>24</v>
-      </c>
-      <c r="K23" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>206</v>
-      </c>
-      <c r="B24" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24">
-        <v>103</v>
-      </c>
-      <c r="E24" t="s">
-        <v>10</v>
-      </c>
-      <c r="F24" t="s">
-        <v>16</v>
-      </c>
-      <c r="G24" t="s">
-        <v>17</v>
-      </c>
-      <c r="H24" t="s">
-        <v>18</v>
-      </c>
-      <c r="I24" t="s">
-        <v>14</v>
-      </c>
-      <c r="J24" t="s">
-        <v>24</v>
-      </c>
-      <c r="K24" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>211</v>
-      </c>
-      <c r="B25" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25">
-        <v>44</v>
-      </c>
-      <c r="E25" t="s">
-        <v>10</v>
-      </c>
-      <c r="F25" t="s">
-        <v>12</v>
-      </c>
-      <c r="G25" t="s">
-        <v>11</v>
-      </c>
-      <c r="H25" t="s">
-        <v>13</v>
-      </c>
-      <c r="I25" t="s">
-        <v>14</v>
-      </c>
-      <c r="J25" t="s">
-        <v>24</v>
-      </c>
-      <c r="K25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>217</v>
-      </c>
-      <c r="B26" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" t="s">
-        <v>67</v>
-      </c>
-      <c r="D26">
-        <v>295</v>
-      </c>
-      <c r="E26" t="s">
-        <v>10</v>
-      </c>
-      <c r="F26" t="s">
-        <v>12</v>
-      </c>
-      <c r="G26" t="s">
-        <v>11</v>
-      </c>
-      <c r="H26" t="s">
-        <v>13</v>
-      </c>
-      <c r="I26" t="s">
-        <v>14</v>
-      </c>
-      <c r="J26" t="s">
-        <v>24</v>
-      </c>
-      <c r="K26" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>229</v>
-      </c>
-      <c r="B27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" t="s">
-        <v>67</v>
-      </c>
-      <c r="D27">
-        <v>191</v>
-      </c>
-      <c r="E27" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" t="s">
-        <v>12</v>
-      </c>
-      <c r="G27" t="s">
-        <v>11</v>
-      </c>
-      <c r="H27" t="s">
-        <v>13</v>
-      </c>
-      <c r="I27" t="s">
-        <v>14</v>
-      </c>
-      <c r="J27" t="s">
-        <v>24</v>
-      </c>
-      <c r="K27" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>230</v>
-      </c>
-      <c r="B28" t="s">
-        <v>62</v>
-      </c>
-      <c r="C28" t="s">
-        <v>67</v>
-      </c>
-      <c r="D28">
-        <v>90</v>
-      </c>
-      <c r="E28" t="s">
-        <v>10</v>
-      </c>
-      <c r="F28" t="s">
-        <v>12</v>
-      </c>
-      <c r="G28" t="s">
-        <v>11</v>
-      </c>
-      <c r="H28" t="s">
-        <v>13</v>
-      </c>
-      <c r="I28" t="s">
-        <v>26</v>
-      </c>
-      <c r="J28" t="s">
-        <v>22</v>
-      </c>
-      <c r="K28" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>220</v>
-      </c>
-      <c r="B29" t="s">
-        <v>52</v>
-      </c>
-      <c r="C29" t="s">
-        <v>67</v>
-      </c>
-      <c r="D29">
-        <v>278</v>
-      </c>
-      <c r="E29" t="s">
-        <v>10</v>
-      </c>
-      <c r="F29" t="s">
-        <v>12</v>
-      </c>
-      <c r="G29" t="s">
-        <v>11</v>
-      </c>
-      <c r="H29" t="s">
-        <v>13</v>
-      </c>
-      <c r="I29" t="s">
-        <v>26</v>
-      </c>
-      <c r="J29" t="s">
-        <v>22</v>
-      </c>
-      <c r="K29" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>214</v>
-      </c>
-      <c r="B30" t="s">
-        <v>46</v>
-      </c>
-      <c r="C30" t="s">
-        <v>67</v>
-      </c>
-      <c r="D30">
-        <v>16</v>
-      </c>
-      <c r="E30" t="s">
-        <v>10</v>
-      </c>
-      <c r="F30" t="s">
-        <v>12</v>
-      </c>
-      <c r="G30" t="s">
-        <v>11</v>
-      </c>
-      <c r="H30" t="s">
-        <v>13</v>
-      </c>
-      <c r="I30" t="s">
-        <v>26</v>
-      </c>
-      <c r="J30" t="s">
-        <v>22</v>
-      </c>
-      <c r="K30" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A33" s="1">
-        <v>196</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D33" s="1">
-        <v>79</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K33" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A34" s="1">
-        <v>225</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D34" s="1">
-        <v>739</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J34" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K34" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A35" s="1">
-        <v>226</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D35" s="1">
-        <v>52</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J35" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K35" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A36" s="1">
-        <v>219</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D36" s="1">
-        <v>65</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J36" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K36" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A37" s="1">
-        <v>216</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D37" s="1">
-        <v>119</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J37" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K37" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A38" s="1">
-        <v>209</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D38" s="1">
-        <v>38</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J38" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K38" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A39" s="1">
-        <v>202</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D39" s="1">
-        <v>42</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J39" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K39" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A40" s="1">
-        <v>203</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D40" s="1">
-        <v>76</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J40" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K40" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A41" s="1">
-        <v>227</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D41" s="1">
-        <v>379</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J41" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K41" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A42" s="1">
-        <v>228</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D42" s="1">
-        <v>45</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J42" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K42" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A43" s="1">
-        <v>210</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D43" s="1">
-        <v>47</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J43" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K43" s="1" t="s">
-        <v>23</v>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D49">
+        <f>SUM(D45:D48)</f>
+        <v>1233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>